<commit_message>
Importing the Processed data files into python
</commit_message>
<xml_diff>
--- a/data/Processed_Data/RailwayInfo.xlsx
+++ b/data/Processed_Data/RailwayInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Academic\Aus_Trains\data\Processed_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB3BC9F-0DF5-4398-87EE-A993387D8517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3C5FD1-02EF-40D4-B8A3-F7117C6D3BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{3AE5864F-F506-40FE-BEF5-325CAB23D357}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3AE5864F-F506-40FE-BEF5-325CAB23D357}"/>
   </bookViews>
   <sheets>
     <sheet name="Stations" sheetId="1" r:id="rId1"/>
@@ -1471,10 +1471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A3C533-154F-42EF-A106-DD2085AC4224}">
-  <dimension ref="A1:F106"/>
+  <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1506,72 +1506,112 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2">
+        <v>151.20500000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3">
+        <v>150.81399999999999</v>
+      </c>
+    </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F4">
-        <v>151.20500000000001</v>
+        <v>150.375</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F5">
-        <v>150.81399999999999</v>
+        <v>149.7209</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
         <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F6">
-        <v>150.375</v>
+        <v>149.26499999999999</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
         <v>44</v>
@@ -1580,78 +1620,78 @@
         <v>52</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F7">
-        <v>149.7209</v>
+        <v>148.911</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
         <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F8">
-        <v>149.26499999999999</v>
+        <v>148.38</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
         <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F9">
-        <v>148.911</v>
+        <v>148.02799999999999</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
         <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F10">
-        <v>148.38</v>
+        <v>147.58699999999999</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
         <v>44</v>
@@ -1660,18 +1700,18 @@
         <v>48</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F11">
-        <v>148.02799999999999</v>
+        <v>147.37</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
         <v>44</v>
@@ -1680,18 +1720,18 @@
         <v>48</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F12">
-        <v>147.58699999999999</v>
+        <v>147.15199999999999</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
         <v>44</v>
@@ -1700,18 +1740,18 @@
         <v>48</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F13">
-        <v>147.37</v>
+        <v>147.036</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
         <v>44</v>
@@ -1720,78 +1760,78 @@
         <v>48</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F14">
-        <v>147.15199999999999</v>
+        <v>146.94999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
         <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F15">
-        <v>147.036</v>
+        <v>146.91999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>124</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>109</v>
       </c>
       <c r="C16" t="s">
         <v>44</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>65</v>
+        <v>139</v>
       </c>
       <c r="F16">
-        <v>146.94999999999999</v>
+        <v>151.09440000000001</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>125</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>110</v>
       </c>
       <c r="C17" t="s">
         <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>66</v>
+        <v>140</v>
       </c>
       <c r="F17">
-        <v>146.91999999999999</v>
+        <v>151.00299999999999</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B18" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C18" t="s">
         <v>44</v>
@@ -1800,78 +1840,78 @@
         <v>49</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F18">
-        <v>151.09440000000001</v>
+        <v>150.69499999999999</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B19" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C19" t="s">
         <v>44</v>
       </c>
       <c r="D19" t="s">
-        <v>49</v>
+        <v>154</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F19">
-        <v>151.00299999999999</v>
+        <v>150.31110000000001</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B20" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C20" t="s">
         <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>49</v>
+        <v>155</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F20">
-        <v>150.69499999999999</v>
+        <v>150.15360000000001</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B21" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C21" t="s">
         <v>44</v>
       </c>
       <c r="D21" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F21">
-        <v>150.31110000000001</v>
+        <v>149.5771</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B22" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C22" t="s">
         <v>44</v>
@@ -1880,18 +1920,18 @@
         <v>155</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F22">
-        <v>150.15360000000001</v>
+        <v>149.24719999999999</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B23" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C23" t="s">
         <v>44</v>
@@ -1900,18 +1940,18 @@
         <v>155</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="F23">
-        <v>149.5771</v>
+        <v>149.1</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B24" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C24" t="s">
         <v>44</v>
@@ -1920,18 +1960,18 @@
         <v>155</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="F24">
-        <v>149.24719999999999</v>
+        <v>148.17500000000001</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B25" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C25" t="s">
         <v>44</v>
@@ -1940,58 +1980,58 @@
         <v>155</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F25">
-        <v>149.1</v>
+        <v>147.15270000000001</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B26" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C26" t="s">
         <v>44</v>
       </c>
       <c r="D26" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F26">
-        <v>148.17500000000001</v>
+        <v>146.64619999999999</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B27" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C27" t="s">
         <v>44</v>
       </c>
       <c r="D27" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F27">
-        <v>147.15270000000001</v>
+        <v>144.30199999999999</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B28" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C28" t="s">
         <v>44</v>
@@ -2000,18 +2040,18 @@
         <v>156</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F28">
-        <v>146.64619999999999</v>
+        <v>143.37970000000001</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B29" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C29" t="s">
         <v>44</v>
@@ -2020,18 +2060,18 @@
         <v>156</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F29">
-        <v>144.30199999999999</v>
+        <v>142.41900000000001</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B30" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C30" t="s">
         <v>44</v>
@@ -2040,118 +2080,118 @@
         <v>156</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F30">
-        <v>143.37970000000001</v>
+        <v>141.45349999999999</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>137</v>
+        <v>197</v>
       </c>
       <c r="B31" t="s">
-        <v>122</v>
+        <v>178</v>
       </c>
       <c r="C31" t="s">
         <v>44</v>
       </c>
       <c r="D31" t="s">
-        <v>156</v>
+        <v>49</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>152</v>
+        <v>221</v>
       </c>
       <c r="F31">
-        <v>142.41900000000001</v>
+        <v>151.0993</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>138</v>
+        <v>198</v>
       </c>
       <c r="B32" t="s">
-        <v>123</v>
+        <v>179</v>
       </c>
       <c r="C32" t="s">
         <v>44</v>
       </c>
       <c r="D32" t="s">
-        <v>156</v>
+        <v>217</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>153</v>
+        <v>222</v>
       </c>
       <c r="F32">
-        <v>141.45349999999999</v>
+        <v>151.34219999999999</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B33" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C33" t="s">
         <v>44</v>
       </c>
       <c r="D33" t="s">
-        <v>49</v>
+        <v>217</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="F33">
-        <v>151.0993</v>
+        <v>151.42099999999999</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B34" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C34" t="s">
         <v>44</v>
       </c>
       <c r="D34" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="F34">
-        <v>151.34219999999999</v>
+        <v>151.583</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B35" t="s">
-        <v>180</v>
+        <v>36</v>
       </c>
       <c r="C35" t="s">
         <v>44</v>
       </c>
       <c r="D35" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="F35">
-        <v>151.42099999999999</v>
+        <v>151.74</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B36" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C36" t="s">
         <v>44</v>
@@ -2160,18 +2200,18 @@
         <v>218</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="F36">
-        <v>151.583</v>
+        <v>151.55099999999999</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>183</v>
       </c>
       <c r="C37" t="s">
         <v>44</v>
@@ -2180,58 +2220,58 @@
         <v>218</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="F37">
-        <v>151.74</v>
+        <v>151.75899999999999</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B38" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C38" t="s">
         <v>44</v>
       </c>
       <c r="D38" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="F38">
-        <v>151.55099999999999</v>
+        <v>151.96299999999999</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B39" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C39" t="s">
         <v>44</v>
       </c>
       <c r="D39" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="F39">
-        <v>151.75899999999999</v>
+        <v>152.374</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B40" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C40" t="s">
         <v>44</v>
@@ -2240,18 +2280,18 @@
         <v>219</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="F40">
-        <v>151.96299999999999</v>
+        <v>152.453</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B41" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C41" t="s">
         <v>44</v>
@@ -2260,18 +2300,18 @@
         <v>219</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="F41">
-        <v>152.374</v>
+        <v>152.71299999999999</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B42" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C42" t="s">
         <v>44</v>
@@ -2280,18 +2320,18 @@
         <v>219</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="F42">
-        <v>152.453</v>
+        <v>152.73099999999999</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B43" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C43" t="s">
         <v>44</v>
@@ -2300,18 +2340,18 @@
         <v>219</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="F43">
-        <v>152.71299999999999</v>
+        <v>152.83500000000001</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B44" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C44" t="s">
         <v>44</v>
@@ -2320,18 +2360,18 @@
         <v>219</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="F44">
-        <v>152.73099999999999</v>
+        <v>152.91900000000001</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B45" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C45" t="s">
         <v>44</v>
@@ -2340,18 +2380,18 @@
         <v>219</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="F45">
-        <v>152.83500000000001</v>
+        <v>153.017</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B46" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C46" t="s">
         <v>44</v>
@@ -2360,18 +2400,18 @@
         <v>219</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F46">
-        <v>152.91900000000001</v>
+        <v>153.101</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B47" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C47" t="s">
         <v>44</v>
@@ -2380,58 +2420,58 @@
         <v>219</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F47">
-        <v>153.017</v>
+        <v>153.11410000000001</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B48" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C48" t="s">
         <v>44</v>
       </c>
       <c r="D48" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="F48">
-        <v>153.101</v>
+        <v>152.93299999999999</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B49" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C49" t="s">
         <v>44</v>
       </c>
       <c r="D49" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="F49">
-        <v>153.11410000000001</v>
+        <v>153.04900000000001</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B50" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C50" t="s">
         <v>44</v>
@@ -2440,98 +2480,98 @@
         <v>220</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F50">
-        <v>152.93299999999999</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>215</v>
-      </c>
-      <c r="B51" t="s">
-        <v>195</v>
-      </c>
-      <c r="C51" t="s">
-        <v>44</v>
-      </c>
-      <c r="D51" t="s">
-        <v>220</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="F51">
-        <v>153.04900000000001</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>216</v>
-      </c>
-      <c r="B52" t="s">
-        <v>196</v>
-      </c>
-      <c r="C52" t="s">
-        <v>44</v>
-      </c>
-      <c r="D52" t="s">
-        <v>220</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="F52">
         <v>153.006</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>242</v>
+      </c>
+      <c r="B55" t="s">
+        <v>243</v>
+      </c>
+      <c r="C55" t="s">
+        <v>241</v>
+      </c>
+      <c r="D55" t="s">
+        <v>244</v>
+      </c>
+      <c r="E55" s="2">
+        <v>-27.4679</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>318</v>
+      </c>
+      <c r="B56" t="s">
+        <v>245</v>
+      </c>
+      <c r="C56" t="s">
+        <v>241</v>
+      </c>
+      <c r="D56" t="s">
+        <v>246</v>
+      </c>
+      <c r="E56" s="2">
+        <v>-27.084700000000002</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>242</v>
+        <v>319</v>
       </c>
       <c r="B57" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="C57" t="s">
         <v>241</v>
       </c>
       <c r="D57" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="E57" s="2">
-        <v>-27.4679</v>
+        <v>-26.8095</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B58" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="C58" t="s">
         <v>241</v>
       </c>
       <c r="D58" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="E58" s="2">
-        <v>-27.084700000000002</v>
+        <v>-26.626799999999999</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B59" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="C59" t="s">
         <v>241</v>
@@ -2540,58 +2580,58 @@
         <v>248</v>
       </c>
       <c r="E59" s="2">
-        <v>-26.8095</v>
+        <v>-26.418600000000001</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B60" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C60" t="s">
         <v>241</v>
       </c>
       <c r="D60" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="E60" s="2">
-        <v>-26.626799999999999</v>
+        <v>-26.158300000000001</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B61" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C61" t="s">
         <v>241</v>
       </c>
       <c r="D61" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="E61" s="2">
-        <v>-26.418600000000001</v>
+        <v>-25.518899999999999</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B62" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C62" t="s">
         <v>241</v>
@@ -2600,18 +2640,18 @@
         <v>252</v>
       </c>
       <c r="E62" s="2">
-        <v>-26.158300000000001</v>
+        <v>-25.319400000000002</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B63" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C63" t="s">
         <v>241</v>
@@ -2620,58 +2660,58 @@
         <v>252</v>
       </c>
       <c r="E63" s="2">
-        <v>-25.518899999999999</v>
+        <v>-24.866199999999999</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B64" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C64" t="s">
         <v>241</v>
       </c>
       <c r="D64" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="E64" s="2">
-        <v>-25.319400000000002</v>
+        <v>-24.3736</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B65" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C65" t="s">
         <v>241</v>
       </c>
       <c r="D65" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="E65" s="2">
-        <v>-24.866199999999999</v>
+        <v>-23.847999999999999</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B66" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C66" t="s">
         <v>241</v>
@@ -2680,198 +2720,198 @@
         <v>257</v>
       </c>
       <c r="E66" s="2">
-        <v>-24.3736</v>
+        <v>-23.795999999999999</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B67" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C67" t="s">
         <v>241</v>
       </c>
       <c r="D67" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="E67" s="2">
-        <v>-23.847999999999999</v>
+        <v>-23.380299999999998</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B68" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C68" t="s">
         <v>241</v>
       </c>
       <c r="D68" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="E68" s="2">
-        <v>-23.795999999999999</v>
+        <v>-22.35</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B69" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="C69" t="s">
         <v>241</v>
       </c>
       <c r="D69" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="E69" s="2">
-        <v>-23.380299999999998</v>
+        <v>-21.906099999999999</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B70" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="C70" t="s">
         <v>241</v>
       </c>
       <c r="D70" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="E70" s="2">
-        <v>-22.35</v>
+        <v>-21.423500000000001</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B71" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C71" t="s">
         <v>241</v>
       </c>
       <c r="D71" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="E71" s="2">
-        <v>-21.906099999999999</v>
+        <v>-21.143999999999998</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B72" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C72" t="s">
         <v>241</v>
       </c>
       <c r="D72" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="E72" s="2">
-        <v>-21.423500000000001</v>
+        <v>-20.401399999999999</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B73" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C73" t="s">
         <v>241</v>
       </c>
       <c r="D73" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="E73" s="2">
-        <v>-21.143999999999998</v>
+        <v>-20.014500000000002</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B74" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C74" t="s">
         <v>241</v>
       </c>
       <c r="D74" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="E74" s="2">
-        <v>-20.401399999999999</v>
+        <v>-19.662500000000001</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B75" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C75" t="s">
         <v>241</v>
       </c>
       <c r="D75" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="E75" s="2">
-        <v>-20.014500000000002</v>
+        <v>-19.573</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B76" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="C76" t="s">
         <v>241</v>
@@ -2880,98 +2920,98 @@
         <v>272</v>
       </c>
       <c r="E76" s="2">
-        <v>-19.662500000000001</v>
+        <v>-19.600000000000001</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B77" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C77" t="s">
         <v>241</v>
       </c>
       <c r="D77" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="E77" s="2">
-        <v>-19.573</v>
+        <v>-19.266400000000001</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B78" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C78" t="s">
         <v>241</v>
       </c>
       <c r="D78" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="E78" s="2">
-        <v>-19.600000000000001</v>
+        <v>-18.648</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B79" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="C79" t="s">
         <v>241</v>
       </c>
       <c r="D79" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="E79" s="2">
-        <v>-19.266400000000001</v>
+        <v>-18.265999999999998</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B80" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C80" t="s">
         <v>241</v>
       </c>
       <c r="D80" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E80" s="2">
-        <v>-18.648</v>
+        <v>-17.932600000000001</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B81" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="C81" t="s">
         <v>241</v>
@@ -2980,284 +3020,284 @@
         <v>280</v>
       </c>
       <c r="E81" s="2">
-        <v>-18.265999999999998</v>
+        <v>-17.525400000000001</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B82" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C82" t="s">
         <v>241</v>
       </c>
       <c r="D82" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="E82" s="2">
-        <v>-17.932600000000001</v>
+        <v>-17.344000000000001</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B83" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C83" t="s">
         <v>241</v>
       </c>
       <c r="D83" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="E83" s="2">
-        <v>-17.525400000000001</v>
+        <v>-17.091000000000001</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B84" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="C84" t="s">
         <v>241</v>
       </c>
       <c r="D84" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="E84" s="2">
-        <v>-17.344000000000001</v>
+        <v>-16.920300000000001</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>345</v>
-      </c>
-      <c r="B85" t="s">
-        <v>285</v>
-      </c>
-      <c r="C85" t="s">
-        <v>241</v>
-      </c>
-      <c r="D85" t="s">
-        <v>284</v>
-      </c>
-      <c r="E85" s="2">
-        <v>-17.091000000000001</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>316</v>
-      </c>
+      <c r="F85" s="1"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>346</v>
-      </c>
-      <c r="B86" t="s">
-        <v>286</v>
-      </c>
-      <c r="C86" t="s">
-        <v>241</v>
-      </c>
-      <c r="D86" t="s">
-        <v>287</v>
-      </c>
-      <c r="E86" s="2">
-        <v>-16.920300000000001</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>317</v>
-      </c>
+      <c r="F86" s="1"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F87" s="1"/>
+      <c r="A87" t="s">
+        <v>39</v>
+      </c>
+      <c r="B87" t="s">
+        <v>35</v>
+      </c>
+      <c r="C87" t="s">
+        <v>45</v>
+      </c>
+      <c r="D87" t="s">
+        <v>68</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F87">
+        <v>144.95249999999999</v>
+      </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F88" s="1"/>
+      <c r="A88" t="s">
+        <v>40</v>
+      </c>
+      <c r="B88" t="s">
+        <v>36</v>
+      </c>
+      <c r="C88" t="s">
+        <v>45</v>
+      </c>
+      <c r="D88" t="s">
+        <v>69</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F88">
+        <v>144.91829999999999</v>
+      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B89" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C89" t="s">
         <v>45</v>
       </c>
       <c r="D89" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F89">
-        <v>144.95249999999999</v>
+        <v>145.1344</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B90" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C90" t="s">
         <v>45</v>
       </c>
       <c r="D90" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F90">
-        <v>144.91829999999999</v>
+        <v>145.9836</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B91" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C91" t="s">
         <v>45</v>
       </c>
       <c r="D91" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F91">
-        <v>145.1344</v>
+        <v>146.3252</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="B92" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="C92" t="s">
         <v>45</v>
       </c>
       <c r="D92" t="s">
-        <v>46</v>
+        <v>95</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="F92">
-        <v>145.9836</v>
+        <v>144.35</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="B93" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="C93" t="s">
         <v>45</v>
       </c>
       <c r="D93" t="s">
-        <v>46</v>
+        <v>96</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="F93">
-        <v>146.3252</v>
+        <v>142.93270000000001</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B94" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C94" t="s">
         <v>45</v>
       </c>
       <c r="D94" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F94">
-        <v>144.35</v>
+        <v>142.77860000000001</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B95" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C95" t="s">
         <v>45</v>
       </c>
       <c r="D95" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F95">
-        <v>142.93270000000001</v>
+        <v>142.19909999999999</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B96" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C96" t="s">
         <v>45</v>
       </c>
       <c r="D96" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F96">
-        <v>142.77860000000001</v>
+        <v>142.03120000000001</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B97" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C97" t="s">
         <v>45</v>
@@ -3266,109 +3306,69 @@
         <v>94</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F97">
-        <v>142.19909999999999</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
-        <v>85</v>
-      </c>
-      <c r="B98" t="s">
-        <v>79</v>
-      </c>
-      <c r="C98" t="s">
-        <v>45</v>
-      </c>
-      <c r="D98" t="s">
-        <v>94</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F98">
-        <v>142.03120000000001</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>86</v>
-      </c>
-      <c r="B99" t="s">
-        <v>80</v>
-      </c>
-      <c r="C99" t="s">
-        <v>45</v>
-      </c>
-      <c r="D99" t="s">
-        <v>94</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F99">
         <v>141.65</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>87</v>
+      </c>
+      <c r="B102" t="s">
+        <v>89</v>
+      </c>
+      <c r="C102" t="s">
+        <v>93</v>
+      </c>
+      <c r="D102" t="s">
+        <v>105</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F102">
+        <v>138.5686</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>88</v>
+      </c>
+      <c r="B103" t="s">
+        <v>90</v>
+      </c>
+      <c r="C103" t="s">
+        <v>93</v>
+      </c>
+      <c r="D103" t="s">
+        <v>104</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F103">
+        <v>139.273</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B104" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C104" t="s">
         <v>93</v>
       </c>
       <c r="D104" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F104">
-        <v>138.5686</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>88</v>
-      </c>
-      <c r="B105" t="s">
-        <v>90</v>
-      </c>
-      <c r="C105" t="s">
-        <v>93</v>
-      </c>
-      <c r="D105" t="s">
-        <v>104</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F105">
-        <v>139.273</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
-        <v>92</v>
-      </c>
-      <c r="B106" t="s">
-        <v>91</v>
-      </c>
-      <c r="C106" t="s">
-        <v>93</v>
-      </c>
-      <c r="D106" t="s">
-        <v>103</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F106">
         <v>140.77000000000001</v>
       </c>
     </row>
@@ -3382,7 +3382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62C6A88F-D5A7-422F-80D3-EFDAF5C3D9C4}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fininshing the data cleaning process
</commit_message>
<xml_diff>
--- a/data/Processed_Data/RailwayInfo.xlsx
+++ b/data/Processed_Data/RailwayInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Academic\Aus_Trains\data\Processed_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3C5FD1-02EF-40D4-B8A3-F7117C6D3BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C54C34-D85F-439E-A205-1978E9A7E18A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3AE5864F-F506-40FE-BEF5-325CAB23D357}"/>
   </bookViews>
@@ -1471,10 +1471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A3C533-154F-42EF-A106-DD2085AC4224}">
-  <dimension ref="A1:F104"/>
+  <dimension ref="A1:F94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="A51" sqref="A51:XFD54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2486,889 +2486,883 @@
         <v>153.006</v>
       </c>
     </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>242</v>
+      </c>
+      <c r="B51" t="s">
+        <v>243</v>
+      </c>
+      <c r="C51" t="s">
+        <v>241</v>
+      </c>
+      <c r="D51" t="s">
+        <v>244</v>
+      </c>
+      <c r="E51" s="2">
+        <v>-27.4679</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>318</v>
+      </c>
+      <c r="B52" t="s">
+        <v>245</v>
+      </c>
+      <c r="C52" t="s">
+        <v>241</v>
+      </c>
+      <c r="D52" t="s">
+        <v>246</v>
+      </c>
+      <c r="E52" s="2">
+        <v>-27.084700000000002</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>319</v>
+      </c>
+      <c r="B53" t="s">
+        <v>247</v>
+      </c>
+      <c r="C53" t="s">
+        <v>241</v>
+      </c>
+      <c r="D53" t="s">
+        <v>248</v>
+      </c>
+      <c r="E53" s="2">
+        <v>-26.8095</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>320</v>
+      </c>
+      <c r="B54" t="s">
+        <v>249</v>
+      </c>
+      <c r="C54" t="s">
+        <v>241</v>
+      </c>
+      <c r="D54" t="s">
+        <v>248</v>
+      </c>
+      <c r="E54" s="2">
+        <v>-26.626799999999999</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>242</v>
+        <v>321</v>
       </c>
       <c r="B55" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="C55" t="s">
         <v>241</v>
       </c>
       <c r="D55" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="E55" s="2">
-        <v>-27.4679</v>
+        <v>-26.418600000000001</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="B56" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="C56" t="s">
         <v>241</v>
       </c>
       <c r="D56" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="E56" s="2">
-        <v>-27.084700000000002</v>
+        <v>-26.158300000000001</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="B57" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="C57" t="s">
         <v>241</v>
       </c>
       <c r="D57" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="E57" s="2">
-        <v>-26.8095</v>
+        <v>-25.518899999999999</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="B58" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="C58" t="s">
         <v>241</v>
       </c>
       <c r="D58" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="E58" s="2">
-        <v>-26.626799999999999</v>
+        <v>-25.319400000000002</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="B59" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="C59" t="s">
         <v>241</v>
       </c>
       <c r="D59" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="E59" s="2">
-        <v>-26.418600000000001</v>
+        <v>-24.866199999999999</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="B60" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="C60" t="s">
         <v>241</v>
       </c>
       <c r="D60" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="E60" s="2">
-        <v>-26.158300000000001</v>
+        <v>-24.3736</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="B61" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="C61" t="s">
         <v>241</v>
       </c>
       <c r="D61" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="E61" s="2">
-        <v>-25.518899999999999</v>
+        <v>-23.847999999999999</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="B62" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="C62" t="s">
         <v>241</v>
       </c>
       <c r="D62" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="E62" s="2">
-        <v>-25.319400000000002</v>
+        <v>-23.795999999999999</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="B63" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="C63" t="s">
         <v>241</v>
       </c>
       <c r="D63" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="E63" s="2">
-        <v>-24.866199999999999</v>
+        <v>-23.380299999999998</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="B64" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="C64" t="s">
         <v>241</v>
       </c>
       <c r="D64" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="E64" s="2">
-        <v>-24.3736</v>
+        <v>-22.35</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="B65" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="C65" t="s">
         <v>241</v>
       </c>
       <c r="D65" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="E65" s="2">
-        <v>-23.847999999999999</v>
+        <v>-21.906099999999999</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="B66" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="C66" t="s">
         <v>241</v>
       </c>
       <c r="D66" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="E66" s="2">
-        <v>-23.795999999999999</v>
+        <v>-21.423500000000001</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="B67" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="C67" t="s">
         <v>241</v>
       </c>
       <c r="D67" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="E67" s="2">
-        <v>-23.380299999999998</v>
+        <v>-21.143999999999998</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="B68" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="C68" t="s">
         <v>241</v>
       </c>
       <c r="D68" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="E68" s="2">
-        <v>-22.35</v>
+        <v>-20.401399999999999</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="B69" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="C69" t="s">
         <v>241</v>
       </c>
       <c r="D69" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="E69" s="2">
-        <v>-21.906099999999999</v>
+        <v>-20.014500000000002</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="B70" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="C70" t="s">
         <v>241</v>
       </c>
       <c r="D70" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="E70" s="2">
-        <v>-21.423500000000001</v>
+        <v>-19.662500000000001</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="B71" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="C71" t="s">
         <v>241</v>
       </c>
       <c r="D71" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="E71" s="2">
-        <v>-21.143999999999998</v>
+        <v>-19.573</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="B72" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="C72" t="s">
         <v>241</v>
       </c>
       <c r="D72" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="E72" s="2">
-        <v>-20.401399999999999</v>
+        <v>-19.600000000000001</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="B73" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="C73" t="s">
         <v>241</v>
       </c>
       <c r="D73" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="E73" s="2">
-        <v>-20.014500000000002</v>
+        <v>-19.266400000000001</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="B74" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="C74" t="s">
         <v>241</v>
       </c>
       <c r="D74" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="E74" s="2">
-        <v>-19.662500000000001</v>
+        <v>-18.648</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="B75" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="C75" t="s">
         <v>241</v>
       </c>
       <c r="D75" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="E75" s="2">
-        <v>-19.573</v>
+        <v>-18.265999999999998</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="B76" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="C76" t="s">
         <v>241</v>
       </c>
       <c r="D76" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="E76" s="2">
-        <v>-19.600000000000001</v>
+        <v>-17.932600000000001</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="B77" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="C77" t="s">
         <v>241</v>
       </c>
       <c r="D77" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="E77" s="2">
-        <v>-19.266400000000001</v>
+        <v>-17.525400000000001</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="B78" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="C78" t="s">
         <v>241</v>
       </c>
       <c r="D78" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="E78" s="2">
-        <v>-18.648</v>
+        <v>-17.344000000000001</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="B79" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="C79" t="s">
         <v>241</v>
       </c>
       <c r="D79" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="E79" s="2">
-        <v>-18.265999999999998</v>
+        <v>-17.091000000000001</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="B80" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="C80" t="s">
         <v>241</v>
       </c>
       <c r="D80" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="E80" s="2">
-        <v>-17.932600000000001</v>
+        <v>-16.920300000000001</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>343</v>
+        <v>39</v>
       </c>
       <c r="B81" t="s">
-        <v>282</v>
+        <v>35</v>
       </c>
       <c r="C81" t="s">
-        <v>241</v>
+        <v>45</v>
       </c>
       <c r="D81" t="s">
-        <v>280</v>
-      </c>
-      <c r="E81" s="2">
-        <v>-17.525400000000001</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>314</v>
+        <v>68</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F81">
+        <v>144.95249999999999</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>344</v>
+        <v>40</v>
       </c>
       <c r="B82" t="s">
-        <v>283</v>
+        <v>36</v>
       </c>
       <c r="C82" t="s">
-        <v>241</v>
+        <v>45</v>
       </c>
       <c r="D82" t="s">
-        <v>284</v>
-      </c>
-      <c r="E82" s="2">
-        <v>-17.344000000000001</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>315</v>
+        <v>69</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F82">
+        <v>144.91829999999999</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>345</v>
+        <v>41</v>
       </c>
       <c r="B83" t="s">
-        <v>285</v>
+        <v>37</v>
       </c>
       <c r="C83" t="s">
-        <v>241</v>
+        <v>45</v>
       </c>
       <c r="D83" t="s">
-        <v>284</v>
-      </c>
-      <c r="E83" s="2">
-        <v>-17.091000000000001</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>316</v>
+        <v>67</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F83">
+        <v>145.1344</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>346</v>
+        <v>42</v>
       </c>
       <c r="B84" t="s">
-        <v>286</v>
+        <v>38</v>
       </c>
       <c r="C84" t="s">
-        <v>241</v>
+        <v>45</v>
       </c>
       <c r="D84" t="s">
-        <v>287</v>
-      </c>
-      <c r="E84" s="2">
-        <v>-16.920300000000001</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>317</v>
+        <v>46</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F84">
+        <v>145.9836</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F85" s="1"/>
+      <c r="A85" t="s">
+        <v>43</v>
+      </c>
+      <c r="B85" t="s">
+        <v>34</v>
+      </c>
+      <c r="C85" t="s">
+        <v>45</v>
+      </c>
+      <c r="D85" t="s">
+        <v>46</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F85">
+        <v>146.3252</v>
+      </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F86" s="1"/>
+      <c r="A86" t="s">
+        <v>81</v>
+      </c>
+      <c r="B86" t="s">
+        <v>75</v>
+      </c>
+      <c r="C86" t="s">
+        <v>45</v>
+      </c>
+      <c r="D86" t="s">
+        <v>95</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F86">
+        <v>144.35</v>
+      </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="B87" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="C87" t="s">
         <v>45</v>
       </c>
       <c r="D87" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="F87">
-        <v>144.95249999999999</v>
+        <v>142.93270000000001</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="B88" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="C88" t="s">
         <v>45</v>
       </c>
       <c r="D88" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="F88">
-        <v>144.91829999999999</v>
+        <v>142.77860000000001</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="B89" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
       <c r="C89" t="s">
         <v>45</v>
       </c>
       <c r="D89" t="s">
-        <v>67</v>
+        <v>94</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="F89">
-        <v>145.1344</v>
+        <v>142.19909999999999</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="B90" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="C90" t="s">
         <v>45</v>
       </c>
       <c r="D90" t="s">
-        <v>46</v>
+        <v>94</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="F90">
-        <v>145.9836</v>
+        <v>142.03120000000001</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="B91" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="C91" t="s">
         <v>45</v>
       </c>
       <c r="D91" t="s">
-        <v>46</v>
+        <v>94</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="F91">
-        <v>146.3252</v>
+        <v>141.65</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B92" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="C92" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="D92" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="F92">
-        <v>144.35</v>
+        <v>138.5686</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B93" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="C93" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="D93" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="F93">
-        <v>142.93270000000001</v>
+        <v>139.273</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C94" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="D94" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="F94">
-        <v>142.77860000000001</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>84</v>
-      </c>
-      <c r="B95" t="s">
-        <v>78</v>
-      </c>
-      <c r="C95" t="s">
-        <v>45</v>
-      </c>
-      <c r="D95" t="s">
-        <v>94</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F95">
-        <v>142.19909999999999</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>85</v>
-      </c>
-      <c r="B96" t="s">
-        <v>79</v>
-      </c>
-      <c r="C96" t="s">
-        <v>45</v>
-      </c>
-      <c r="D96" t="s">
-        <v>94</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F96">
-        <v>142.03120000000001</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>86</v>
-      </c>
-      <c r="B97" t="s">
-        <v>80</v>
-      </c>
-      <c r="C97" t="s">
-        <v>45</v>
-      </c>
-      <c r="D97" t="s">
-        <v>94</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F97">
-        <v>141.65</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>87</v>
-      </c>
-      <c r="B102" t="s">
-        <v>89</v>
-      </c>
-      <c r="C102" t="s">
-        <v>93</v>
-      </c>
-      <c r="D102" t="s">
-        <v>105</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F102">
-        <v>138.5686</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>88</v>
-      </c>
-      <c r="B103" t="s">
-        <v>90</v>
-      </c>
-      <c r="C103" t="s">
-        <v>93</v>
-      </c>
-      <c r="D103" t="s">
-        <v>104</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F103">
-        <v>139.273</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
-        <v>92</v>
-      </c>
-      <c r="B104" t="s">
-        <v>91</v>
-      </c>
-      <c r="C104" t="s">
-        <v>93</v>
-      </c>
-      <c r="D104" t="s">
-        <v>103</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F104">
         <v>140.77000000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Creating the location markers
</commit_message>
<xml_diff>
--- a/data/Processed_Data/RailwayInfo.xlsx
+++ b/data/Processed_Data/RailwayInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Academic\Aus_Trains\data\Processed_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C54C34-D85F-439E-A205-1978E9A7E18A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7ED51A-6CA2-4446-8CEB-6AA17A6F7A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3AE5864F-F506-40FE-BEF5-325CAB23D357}"/>
+    <workbookView xWindow="6960" yWindow="3300" windowWidth="17280" windowHeight="8880" xr2:uid="{3AE5864F-F506-40FE-BEF5-325CAB23D357}"/>
   </bookViews>
   <sheets>
     <sheet name="Stations" sheetId="1" r:id="rId1"/>
@@ -1474,7 +1474,7 @@
   <dimension ref="A1:F94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51:XFD54"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Creating the railway line of the overland
</commit_message>
<xml_diff>
--- a/data/Processed_Data/RailwayInfo.xlsx
+++ b/data/Processed_Data/RailwayInfo.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Academic\Aus_Trains\data\Processed_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7ED51A-6CA2-4446-8CEB-6AA17A6F7A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7CCEFA-57A3-49A0-A353-C8F18DC11ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6960" yWindow="3300" windowWidth="17280" windowHeight="8880" xr2:uid="{3AE5864F-F506-40FE-BEF5-325CAB23D357}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{3AE5864F-F506-40FE-BEF5-325CAB23D357}"/>
   </bookViews>
   <sheets>
     <sheet name="Stations" sheetId="1" r:id="rId1"/>
-    <sheet name="TrainServices" sheetId="2" r:id="rId2"/>
+    <sheet name="Overland Line" sheetId="3" r:id="rId2"/>
+    <sheet name="TrainServices" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="352">
   <si>
     <t>Station_ID</t>
   </si>
@@ -93,9 +94,6 @@
     <t>Gunning Station</t>
   </si>
   <si>
-    <t>Yass Junction</t>
-  </si>
-  <si>
     <t>Harden Station</t>
   </si>
   <si>
@@ -408,9 +406,6 @@
     <t>Menindee Station</t>
   </si>
   <si>
-    <t>Broken Hill</t>
-  </si>
-  <si>
     <t>NSW_15</t>
   </si>
   <si>
@@ -573,18 +568,6 @@
     <t>Sydney - Broken-hill</t>
   </si>
   <si>
-    <t xml:space="preserve">Hornsby </t>
-  </si>
-  <si>
-    <t>Gosford</t>
-  </si>
-  <si>
-    <t>Wyong</t>
-  </si>
-  <si>
-    <t>Fassifern</t>
-  </si>
-  <si>
     <t>Maitland</t>
   </si>
   <si>
@@ -1090,6 +1073,27 @@
   </si>
   <si>
     <t>Brisbane - Cairns</t>
+  </si>
+  <si>
+    <t>Yass Junction station</t>
+  </si>
+  <si>
+    <t>Broken Hill station</t>
+  </si>
+  <si>
+    <t>Hornsby station</t>
+  </si>
+  <si>
+    <t>Gosford station</t>
+  </si>
+  <si>
+    <t>Wyong station</t>
+  </si>
+  <si>
+    <t>Fassifern station</t>
+  </si>
+  <si>
+    <t>Order</t>
   </si>
 </sst>
 </file>
@@ -1473,8 +1477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A3C533-154F-42EF-A106-DD2085AC4224}">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86:B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1514,13 +1518,13 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F2">
         <v>151.20500000000001</v>
@@ -1534,13 +1538,13 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3">
         <v>150.81399999999999</v>
@@ -1554,13 +1558,13 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F4">
         <v>150.375</v>
@@ -1574,13 +1578,13 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F5">
         <v>149.7209</v>
@@ -1594,13 +1598,13 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F6">
         <v>149.26499999999999</v>
@@ -1611,16 +1615,16 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>345</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F7">
         <v>148.911</v>
@@ -1631,16 +1635,16 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F8">
         <v>148.38</v>
@@ -1648,19 +1652,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F9">
         <v>148.02799999999999</v>
@@ -1668,19 +1672,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F10">
         <v>147.58699999999999</v>
@@ -1688,19 +1692,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F11">
         <v>147.37</v>
@@ -1708,19 +1712,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F12">
         <v>147.15199999999999</v>
@@ -1728,19 +1732,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F13">
         <v>147.036</v>
@@ -1748,19 +1752,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F14">
         <v>146.94999999999999</v>
@@ -1768,19 +1772,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F15">
         <v>146.91999999999999</v>
@@ -1788,19 +1792,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F16">
         <v>151.09440000000001</v>
@@ -1808,19 +1812,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F17">
         <v>151.00299999999999</v>
@@ -1828,19 +1832,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F18">
         <v>150.69499999999999</v>
@@ -1848,19 +1852,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F19">
         <v>150.31110000000001</v>
@@ -1868,19 +1872,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D20" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F20">
         <v>150.15360000000001</v>
@@ -1888,19 +1892,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F21">
         <v>149.5771</v>
@@ -1908,19 +1912,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D22" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F22">
         <v>149.24719999999999</v>
@@ -1928,19 +1932,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F23">
         <v>149.1</v>
@@ -1948,19 +1952,19 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D24" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F24">
         <v>148.17500000000001</v>
@@ -1968,19 +1972,19 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F25">
         <v>147.15270000000001</v>
@@ -1988,19 +1992,19 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D26" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F26">
         <v>146.64619999999999</v>
@@ -2008,19 +2012,19 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D27" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F27">
         <v>144.30199999999999</v>
@@ -2028,19 +2032,19 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D28" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F28">
         <v>143.37970000000001</v>
@@ -2048,19 +2052,19 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D29" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F29">
         <v>142.41900000000001</v>
@@ -2068,19 +2072,19 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B30" t="s">
-        <v>123</v>
+        <v>346</v>
       </c>
       <c r="C30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D30" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F30">
         <v>141.45349999999999</v>
@@ -2088,19 +2092,19 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B31" t="s">
-        <v>178</v>
+        <v>347</v>
       </c>
       <c r="C31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="F31">
         <v>151.0993</v>
@@ -2108,19 +2112,19 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B32" t="s">
-        <v>179</v>
+        <v>348</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D32" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F32">
         <v>151.34219999999999</v>
@@ -2128,19 +2132,19 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B33" t="s">
-        <v>180</v>
+        <v>349</v>
       </c>
       <c r="C33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D33" t="s">
+        <v>211</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>223</v>
       </c>
       <c r="F33">
         <v>151.42099999999999</v>
@@ -2148,19 +2152,19 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B34" t="s">
-        <v>181</v>
+        <v>350</v>
       </c>
       <c r="C34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D34" t="s">
+        <v>212</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>224</v>
       </c>
       <c r="F34">
         <v>151.583</v>
@@ -2168,19 +2172,19 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D35" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="F35">
         <v>151.74</v>
@@ -2188,19 +2192,19 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B36" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D36" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="F36">
         <v>151.55099999999999</v>
@@ -2208,19 +2212,19 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B37" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D37" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="F37">
         <v>151.75899999999999</v>
@@ -2228,19 +2232,19 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B38" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D38" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="F38">
         <v>151.96299999999999</v>
@@ -2248,19 +2252,19 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B39" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D39" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F39">
         <v>152.374</v>
@@ -2268,19 +2272,19 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B40" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="C40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D40" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="F40">
         <v>152.453</v>
@@ -2288,19 +2292,19 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B41" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="C41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D41" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="F41">
         <v>152.71299999999999</v>
@@ -2308,19 +2312,19 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B42" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D42" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="F42">
         <v>152.73099999999999</v>
@@ -2328,19 +2332,19 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B43" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D43" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="F43">
         <v>152.83500000000001</v>
@@ -2348,19 +2352,19 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B44" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D44" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="F44">
         <v>152.91900000000001</v>
@@ -2368,19 +2372,19 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B45" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D45" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="F45">
         <v>153.017</v>
@@ -2388,19 +2392,19 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B46" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="C46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D46" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="F46">
         <v>153.101</v>
@@ -2408,19 +2412,19 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>207</v>
+      </c>
+      <c r="B47" t="s">
+        <v>187</v>
+      </c>
+      <c r="C47" t="s">
+        <v>43</v>
+      </c>
+      <c r="D47" t="s">
         <v>213</v>
       </c>
-      <c r="B47" t="s">
-        <v>193</v>
-      </c>
-      <c r="C47" t="s">
-        <v>44</v>
-      </c>
-      <c r="D47" t="s">
-        <v>219</v>
-      </c>
       <c r="E47" s="1" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="F47">
         <v>153.11410000000001</v>
@@ -2428,19 +2432,19 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>208</v>
+      </c>
+      <c r="B48" t="s">
+        <v>188</v>
+      </c>
+      <c r="C48" t="s">
+        <v>43</v>
+      </c>
+      <c r="D48" t="s">
         <v>214</v>
       </c>
-      <c r="B48" t="s">
-        <v>194</v>
-      </c>
-      <c r="C48" t="s">
-        <v>44</v>
-      </c>
-      <c r="D48" t="s">
-        <v>220</v>
-      </c>
       <c r="E48" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="F48">
         <v>152.93299999999999</v>
@@ -2448,19 +2452,19 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B49" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D49" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="F49">
         <v>153.04900000000001</v>
@@ -2468,19 +2472,19 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B50" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C50" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D50" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F50">
         <v>153.006</v>
@@ -2488,619 +2492,619 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B51" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C51" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D51" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="E51" s="2">
         <v>-27.4679</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="B52" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C52" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D52" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="E52" s="2">
         <v>-27.084700000000002</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="B53" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C53" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D53" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="E53" s="2">
         <v>-26.8095</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="B54" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C54" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D54" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="E54" s="2">
         <v>-26.626799999999999</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="B55" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C55" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D55" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="E55" s="2">
         <v>-26.418600000000001</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B56" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C56" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D56" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="E56" s="2">
         <v>-26.158300000000001</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="B57" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C57" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D57" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="E57" s="2">
         <v>-25.518899999999999</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="B58" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C58" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D58" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="E58" s="2">
         <v>-25.319400000000002</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="B59" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C59" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D59" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="E59" s="2">
         <v>-24.866199999999999</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="B60" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C60" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D60" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="E60" s="2">
         <v>-24.3736</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="B61" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="C61" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D61" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="E61" s="2">
         <v>-23.847999999999999</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="B62" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="C62" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D62" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="E62" s="2">
         <v>-23.795999999999999</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="B63" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="C63" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D63" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="E63" s="2">
         <v>-23.380299999999998</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="B64" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="C64" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D64" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E64" s="2">
         <v>-22.35</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="B65" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C65" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D65" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E65" s="2">
         <v>-21.906099999999999</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="B66" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C66" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D66" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="E66" s="2">
         <v>-21.423500000000001</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="B67" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C67" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D67" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="E67" s="2">
         <v>-21.143999999999998</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="B68" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C68" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D68" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="E68" s="2">
         <v>-20.401399999999999</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="B69" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C69" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D69" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="E69" s="2">
         <v>-20.014500000000002</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="B70" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="C70" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D70" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="E70" s="2">
         <v>-19.662500000000001</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="B71" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="C71" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D71" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="E71" s="2">
         <v>-19.573</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="B72" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="C72" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D72" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="E72" s="2">
         <v>-19.600000000000001</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="B73" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C73" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D73" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="E73" s="2">
         <v>-19.266400000000001</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="B74" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="C74" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D74" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="E74" s="2">
         <v>-18.648</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="B75" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="C75" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D75" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="E75" s="2">
         <v>-18.265999999999998</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="B76" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="C76" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D76" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="E76" s="2">
         <v>-17.932600000000001</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="B77" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="C77" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D77" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="E77" s="2">
         <v>-17.525400000000001</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="B78" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="C78" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D78" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E78" s="2">
         <v>-17.344000000000001</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="B79" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="C79" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D79" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E79" s="2">
         <v>-17.091000000000001</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="B80" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="C80" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D80" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E80" s="2">
         <v>-16.920300000000001</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B81" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C81" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D81" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F81">
         <v>144.95249999999999</v>
@@ -3108,19 +3112,19 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B82" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C82" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D82" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F82">
         <v>144.91829999999999</v>
@@ -3128,19 +3132,19 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B83" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C83" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D83" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F83">
         <v>145.1344</v>
@@ -3148,19 +3152,19 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B84" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C84" t="s">
+        <v>44</v>
+      </c>
+      <c r="D84" t="s">
         <v>45</v>
       </c>
-      <c r="D84" t="s">
-        <v>46</v>
-      </c>
       <c r="E84" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F84">
         <v>145.9836</v>
@@ -3168,19 +3172,19 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B85" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C85" t="s">
+        <v>44</v>
+      </c>
+      <c r="D85" t="s">
         <v>45</v>
       </c>
-      <c r="D85" t="s">
-        <v>46</v>
-      </c>
       <c r="E85" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F85">
         <v>146.3252</v>
@@ -3188,19 +3192,19 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B86" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C86" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D86" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F86">
         <v>144.35</v>
@@ -3208,19 +3212,19 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B87" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C87" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F87">
         <v>142.93270000000001</v>
@@ -3228,19 +3232,19 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B88" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C88" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D88" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F88">
         <v>142.77860000000001</v>
@@ -3248,19 +3252,19 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B89" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C89" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D89" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F89">
         <v>142.19909999999999</v>
@@ -3268,19 +3272,19 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B90" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C90" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D90" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F90">
         <v>142.03120000000001</v>
@@ -3288,19 +3292,19 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B91" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C91" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D91" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F91">
         <v>141.65</v>
@@ -3308,19 +3312,19 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B92" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C92" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D92" t="s">
+        <v>104</v>
+      </c>
+      <c r="E92" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="F92">
         <v>138.5686</v>
@@ -3328,19 +3332,19 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B93" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C93" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D93" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F93">
         <v>139.273</v>
@@ -3348,19 +3352,19 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
+        <v>91</v>
+      </c>
+      <c r="B94" t="s">
+        <v>90</v>
+      </c>
+      <c r="C94" t="s">
         <v>92</v>
       </c>
-      <c r="B94" t="s">
-        <v>91</v>
-      </c>
-      <c r="C94" t="s">
-        <v>93</v>
-      </c>
       <c r="D94" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F94">
         <v>140.77000000000001</v>
@@ -3373,6 +3377,112 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A80D763E-E741-44C5-829C-E5A7A570CA40}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62C6A88F-D5A7-422F-80D3-EFDAF5C3D9C4}">
   <dimension ref="A1:H6"/>
   <sheetViews>
@@ -3391,42 +3501,42 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" t="s">
         <v>157</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>158</v>
       </c>
-      <c r="C1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D1" t="s">
-        <v>160</v>
-      </c>
       <c r="E1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1" t="s">
         <v>169</v>
       </c>
-      <c r="F1" t="s">
-        <v>170</v>
-      </c>
-      <c r="G1" t="s">
-        <v>171</v>
-      </c>
       <c r="H1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D2" t="s">
         <v>166</v>
-      </c>
-      <c r="C2" t="s">
-        <v>167</v>
-      </c>
-      <c r="D2" t="s">
-        <v>168</v>
       </c>
       <c r="E2">
         <v>10.5</v>
@@ -3443,16 +3553,16 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D3" t="s">
         <v>172</v>
-      </c>
-      <c r="C3" t="s">
-        <v>173</v>
-      </c>
-      <c r="D3" t="s">
-        <v>174</v>
       </c>
       <c r="E3">
         <v>10.5</v>
@@ -3469,16 +3579,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E4">
         <v>13</v>
@@ -3495,16 +3605,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" t="s">
         <v>164</v>
       </c>
-      <c r="B5" t="s">
-        <v>166</v>
-      </c>
       <c r="C5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D5" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="E5">
         <v>14</v>
@@ -3521,16 +3631,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B6" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="C6" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="D6" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="E6">
         <v>25</v>

</xml_diff>

<commit_message>
Creation of the overland line and the creation of the Spirit of QLD line.
</commit_message>
<xml_diff>
--- a/data/Processed_Data/RailwayInfo.xlsx
+++ b/data/Processed_Data/RailwayInfo.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Academic\Aus_Trains\data\Processed_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7CCEFA-57A3-49A0-A353-C8F18DC11ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41B358B-6574-4D70-8A72-86D2B8DAD416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{3AE5864F-F506-40FE-BEF5-325CAB23D357}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{3AE5864F-F506-40FE-BEF5-325CAB23D357}"/>
   </bookViews>
   <sheets>
     <sheet name="Stations" sheetId="1" r:id="rId1"/>
-    <sheet name="Overland Line" sheetId="3" r:id="rId2"/>
-    <sheet name="TrainServices" sheetId="2" r:id="rId3"/>
+    <sheet name="Spirit of QLD" sheetId="5" r:id="rId2"/>
+    <sheet name="Overland Line" sheetId="3" r:id="rId3"/>
+    <sheet name="TrainServices" sheetId="2" r:id="rId4"/>
+    <sheet name="XPT1" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="352">
   <si>
     <t>Station_ID</t>
   </si>
@@ -1477,8 +1479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A3C533-154F-42EF-A106-DD2085AC4224}">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86:B94"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51:B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3377,10 +3379,276 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37280570-26AA-4C78-B7A9-EB280A4BCB69}">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>241</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>243</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>244</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>245</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>247</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>248</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>250</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>252</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>253</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>254</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>256</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>258</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>259</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>261</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>262</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>264</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>265</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>267</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>268</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>269</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>271</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>273</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>275</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>276</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>277</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>279</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>280</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A80D763E-E741-44C5-829C-E5A7A570CA40}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -3482,12 +3750,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62C6A88F-D5A7-422F-80D3-EFDAF5C3D9C4}">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3659,4 +3927,185 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46246001-2BB8-4225-84EA-8FF4EF6BB838}">
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>345</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:B20">
+    <sortCondition ref="B3:B20"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>